<commit_message>
Update the data driven
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,16 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668CD5C4-B5D9-428D-93BE-17022AA5E777}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{62E69CFB-7DE1-4EE7-A3D9-3D8132AC9AC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18384" windowHeight="3480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:Q10"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>Component</t>
   </si>
@@ -62,6 +64,27 @@
   </si>
   <si>
     <t>Test Description</t>
+  </si>
+  <si>
+    <t>Method Interceptors</t>
+  </si>
+  <si>
+    <t>6.9.13.4</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>Test Bug Summary</t>
+  </si>
+  <si>
+    <t>Bug Test Description</t>
+  </si>
+  <si>
+    <t>Linux</t>
+  </si>
+  <si>
+    <t>Macintosh</t>
   </si>
 </sst>
 </file>
@@ -381,7 +404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -466,4 +489,97 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0BC711D-3911-4CDB-B520-0D89A970B2DB}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>